<commit_message>
Added data notes about files uploaded on 2/17/16
</commit_message>
<xml_diff>
--- a/WIT4 Data notes.xlsx
+++ b/WIT4 Data notes.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17540" tabRatio="500"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="21">
   <si>
     <t>Subject</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>Run with wrong Eprime program (BG from Joe's study 2)- not usable, didn't upload to git</t>
+  </si>
+  <si>
+    <t>Says sub 57 in data file (but not file name), needs to be changed to sub 58</t>
   </si>
 </sst>
 </file>
@@ -143,8 +146,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -165,17 +170,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -505,10 +512,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -968,6 +975,393 @@
         <v>9</v>
       </c>
     </row>
+    <row r="38" spans="1:4">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>4</v>
+      </c>
+      <c r="D38" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>5</v>
+      </c>
+      <c r="D39" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>4</v>
+      </c>
+      <c r="D40" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>5</v>
+      </c>
+      <c r="D41" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>4</v>
+      </c>
+      <c r="D42" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>5</v>
+      </c>
+      <c r="D43" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>4</v>
+      </c>
+      <c r="D44" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>5</v>
+      </c>
+      <c r="D45" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>4</v>
+      </c>
+      <c r="D46" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>4</v>
+      </c>
+      <c r="D47" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>5</v>
+      </c>
+      <c r="D48" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>4</v>
+      </c>
+      <c r="D49" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>5</v>
+      </c>
+      <c r="D50" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>4</v>
+      </c>
+      <c r="D51" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>5</v>
+      </c>
+      <c r="D52" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>4</v>
+      </c>
+      <c r="D53" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>5</v>
+      </c>
+      <c r="D54" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>4</v>
+      </c>
+      <c r="D55" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>5</v>
+      </c>
+      <c r="D56" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>4</v>
+      </c>
+      <c r="D57" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>4</v>
+      </c>
+      <c r="D58" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>5</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D59" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>5</v>
+      </c>
+      <c r="D60" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>4</v>
+      </c>
+      <c r="D61" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1">
+      <c r="A67">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1">
+      <c r="A69">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1">
+      <c r="A70">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1">
+      <c r="A71">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1">
+      <c r="A72">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1">
+      <c r="A73">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1">
+      <c r="A74">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1">
+      <c r="A75">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1">
+      <c r="A76">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1">
+      <c r="A77">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1">
+      <c r="A78">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1">
+      <c r="A79">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1">
+      <c r="A80">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1">
+      <c r="A81">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1">
+      <c r="A82">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1">
+      <c r="A83">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1">
+      <c r="A84">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1">
+      <c r="A85">
+        <v>84</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Updated data collection notes, deleted unnecessary files
</commit_message>
<xml_diff>
--- a/WIT4 Data notes.xlsx
+++ b/WIT4 Data notes.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17540" tabRatio="500"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="25">
   <si>
     <t>Subject</t>
   </si>
@@ -51,9 +51,6 @@
     <t>X</t>
   </si>
   <si>
-    <t>for last 20 trials, only pressed j</t>
-  </si>
-  <si>
     <t>No data file</t>
   </si>
   <si>
@@ -81,7 +78,22 @@
     <t>Run with wrong Eprime program (BG from Joe's study 2)- not usable, didn't upload to git</t>
   </si>
   <si>
-    <t>Says sub 57 in data file (but not file name), needs to be changed to sub 58</t>
+    <t>Filename is ...GT-162-2.edat2</t>
+  </si>
+  <si>
+    <t>For some reason, there's a second 74 (so we have an extra subject?) Could be that experimenter didn't write down first 74, so next experimenter ran a second 74. Filename is …GT-74-2.edat2</t>
+  </si>
+  <si>
+    <t>Says sub 57 in data file (file name is …GN-58-1.edat2), sub num in data file needs to be changed to sub 58</t>
+  </si>
+  <si>
+    <t>Filename is …GT-74-2.edat2</t>
+  </si>
+  <si>
+    <t>Subject number is wrong (77)- in file name and data file (filename is …GT-77-1.edat2)</t>
+  </si>
+  <si>
+    <t>Filename is ...GN-77-1.edat2</t>
   </si>
 </sst>
 </file>
@@ -512,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D85"/>
+  <dimension ref="A1:D107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C60" sqref="C60"/>
+    <sheetView tabSelected="1" topLeftCell="A74" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C80" sqref="C80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -584,7 +596,7 @@
         <v>5</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
         <v>8</v>
@@ -633,9 +645,6 @@
       <c r="B9" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="D9" t="s">
         <v>9</v>
       </c>
@@ -670,7 +679,7 @@
         <v>4</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D12" t="s">
         <v>8</v>
@@ -706,7 +715,7 @@
         <v>5</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D15" t="s">
         <v>9</v>
@@ -720,7 +729,7 @@
         <v>4</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D16" t="s">
         <v>9</v>
@@ -734,7 +743,7 @@
         <v>5</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D17" t="s">
         <v>9</v>
@@ -770,7 +779,7 @@
         <v>5</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D20" t="s">
         <v>9</v>
@@ -916,7 +925,7 @@
         <v>5</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D33" t="s">
         <v>9</v>
@@ -941,7 +950,7 @@
         <v>4</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D35" t="s">
         <v>9</v>
@@ -955,7 +964,7 @@
         <v>4</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D36" t="s">
         <v>8</v>
@@ -969,7 +978,7 @@
         <v>4</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D37" t="s">
         <v>9</v>
@@ -1206,7 +1215,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:4" ht="30">
       <c r="A59">
         <v>58</v>
       </c>
@@ -1214,7 +1223,7 @@
         <v>5</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D59" t="s">
         <v>9</v>
@@ -1246,120 +1255,518 @@
       <c r="A62">
         <v>61</v>
       </c>
+      <c r="B62" t="s">
+        <v>5</v>
+      </c>
+      <c r="D62" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63">
         <v>62</v>
       </c>
+      <c r="B63" t="s">
+        <v>4</v>
+      </c>
+      <c r="D63" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="64" spans="1:4">
       <c r="A64">
         <v>63</v>
       </c>
-    </row>
-    <row r="65" spans="1:1">
+      <c r="B64" t="s">
+        <v>5</v>
+      </c>
+      <c r="D64" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
       <c r="A65">
         <v>64</v>
       </c>
-    </row>
-    <row r="66" spans="1:1">
+      <c r="B65" t="s">
+        <v>4</v>
+      </c>
+      <c r="D65" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
       <c r="A66">
         <v>65</v>
       </c>
-    </row>
-    <row r="67" spans="1:1">
+      <c r="B66" t="s">
+        <v>5</v>
+      </c>
+      <c r="D66" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
       <c r="A67">
         <v>66</v>
       </c>
-    </row>
-    <row r="68" spans="1:1">
+      <c r="B67" t="s">
+        <v>5</v>
+      </c>
+      <c r="D67" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
       <c r="A68">
         <v>67</v>
       </c>
-    </row>
-    <row r="69" spans="1:1">
+      <c r="B68" t="s">
+        <v>5</v>
+      </c>
+      <c r="D68" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
       <c r="A69">
         <v>68</v>
       </c>
-    </row>
-    <row r="70" spans="1:1">
+      <c r="B69" t="s">
+        <v>4</v>
+      </c>
+      <c r="D69" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
       <c r="A70">
         <v>69</v>
       </c>
-    </row>
-    <row r="71" spans="1:1">
+      <c r="B70" t="s">
+        <v>5</v>
+      </c>
+      <c r="D70" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
       <c r="A71">
         <v>70</v>
       </c>
-    </row>
-    <row r="72" spans="1:1">
+      <c r="B71" t="s">
+        <v>4</v>
+      </c>
+      <c r="D71" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
       <c r="A72">
         <v>71</v>
       </c>
-    </row>
-    <row r="73" spans="1:1">
+      <c r="B72" t="s">
+        <v>5</v>
+      </c>
+      <c r="D72" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
       <c r="A73">
         <v>72</v>
       </c>
-    </row>
-    <row r="74" spans="1:1">
+      <c r="B73" t="s">
+        <v>4</v>
+      </c>
+      <c r="D73" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
       <c r="A74">
         <v>73</v>
       </c>
-    </row>
-    <row r="75" spans="1:1">
+      <c r="B74" t="s">
+        <v>5</v>
+      </c>
+      <c r="D74" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
       <c r="A75">
         <v>74</v>
       </c>
-    </row>
-    <row r="76" spans="1:1">
+      <c r="B75" t="s">
+        <v>4</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D75" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="45">
       <c r="A76">
+        <v>74</v>
+      </c>
+      <c r="B76" t="s">
+        <v>4</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77">
         <v>75</v>
       </c>
-    </row>
-    <row r="77" spans="1:1">
-      <c r="A77">
+      <c r="B77" t="s">
+        <v>5</v>
+      </c>
+      <c r="D77" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" ht="30">
+      <c r="A78">
         <v>76</v>
       </c>
-    </row>
-    <row r="78" spans="1:1">
-      <c r="A78">
+      <c r="B78" t="s">
+        <v>4</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D78" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79">
         <v>77</v>
       </c>
-    </row>
-    <row r="79" spans="1:1">
-      <c r="A79">
+      <c r="B79" t="s">
+        <v>5</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D79" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="A80">
         <v>78</v>
       </c>
-    </row>
-    <row r="80" spans="1:1">
-      <c r="A80">
+      <c r="B80" t="s">
+        <v>4</v>
+      </c>
+      <c r="D80" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="A81">
         <v>79</v>
       </c>
-    </row>
-    <row r="81" spans="1:1">
-      <c r="A81">
+      <c r="B81" t="s">
+        <v>5</v>
+      </c>
+      <c r="D81" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
+      <c r="A82">
         <v>80</v>
       </c>
-    </row>
-    <row r="82" spans="1:1">
-      <c r="A82">
+      <c r="B82" t="s">
+        <v>4</v>
+      </c>
+      <c r="D82" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
+      <c r="A83">
         <v>81</v>
       </c>
-    </row>
-    <row r="83" spans="1:1">
-      <c r="A83">
+      <c r="B83" t="s">
+        <v>5</v>
+      </c>
+      <c r="D83" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
+      <c r="A84">
         <v>82</v>
       </c>
-    </row>
-    <row r="84" spans="1:1">
-      <c r="A84">
+      <c r="B84" t="s">
+        <v>4</v>
+      </c>
+      <c r="D84" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
+      <c r="A85">
         <v>83</v>
       </c>
-    </row>
-    <row r="85" spans="1:1">
-      <c r="A85">
+      <c r="B85" t="s">
+        <v>5</v>
+      </c>
+      <c r="D85" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4">
+      <c r="A86">
         <v>84</v>
+      </c>
+      <c r="B86" t="s">
+        <v>4</v>
+      </c>
+      <c r="D86" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4">
+      <c r="A87">
+        <v>85</v>
+      </c>
+      <c r="B87" t="s">
+        <v>5</v>
+      </c>
+      <c r="D87" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4">
+      <c r="A88">
+        <v>86</v>
+      </c>
+      <c r="B88" t="s">
+        <v>4</v>
+      </c>
+      <c r="D88" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4">
+      <c r="A89">
+        <v>87</v>
+      </c>
+      <c r="B89" t="s">
+        <v>5</v>
+      </c>
+      <c r="D89" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
+      <c r="A90">
+        <v>88</v>
+      </c>
+      <c r="B90" t="s">
+        <v>4</v>
+      </c>
+      <c r="D90" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
+      <c r="A91">
+        <v>89</v>
+      </c>
+      <c r="B91" t="s">
+        <v>5</v>
+      </c>
+      <c r="D91" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4">
+      <c r="A92">
+        <v>90</v>
+      </c>
+      <c r="B92" t="s">
+        <v>4</v>
+      </c>
+      <c r="D92" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4">
+      <c r="A93">
+        <v>91</v>
+      </c>
+      <c r="B93" t="s">
+        <v>5</v>
+      </c>
+      <c r="D93" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4">
+      <c r="A94">
+        <v>92</v>
+      </c>
+      <c r="B94" t="s">
+        <v>5</v>
+      </c>
+      <c r="D94" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4">
+      <c r="A95">
+        <v>93</v>
+      </c>
+      <c r="B95" t="s">
+        <v>4</v>
+      </c>
+      <c r="D95" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4">
+      <c r="A96">
+        <v>94</v>
+      </c>
+      <c r="B96" t="s">
+        <v>5</v>
+      </c>
+      <c r="D96" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4">
+      <c r="A97">
+        <v>95</v>
+      </c>
+      <c r="B97" t="s">
+        <v>4</v>
+      </c>
+      <c r="D97" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4">
+      <c r="A98">
+        <v>96</v>
+      </c>
+      <c r="B98" t="s">
+        <v>5</v>
+      </c>
+      <c r="D98" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4">
+      <c r="A99">
+        <v>97</v>
+      </c>
+      <c r="B99" t="s">
+        <v>4</v>
+      </c>
+      <c r="D99" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4">
+      <c r="A100">
+        <v>98</v>
+      </c>
+      <c r="B100" t="s">
+        <v>5</v>
+      </c>
+      <c r="D100" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4">
+      <c r="A101">
+        <v>99</v>
+      </c>
+      <c r="B101" t="s">
+        <v>4</v>
+      </c>
+      <c r="D101" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4">
+      <c r="A102">
+        <v>100</v>
+      </c>
+      <c r="B102" t="s">
+        <v>5</v>
+      </c>
+      <c r="D102" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4">
+      <c r="A103">
+        <v>101</v>
+      </c>
+      <c r="B103" t="s">
+        <v>4</v>
+      </c>
+      <c r="D103" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4">
+      <c r="A104">
+        <v>102</v>
+      </c>
+      <c r="B104" t="s">
+        <v>4</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D104" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4">
+      <c r="A105">
+        <v>103</v>
+      </c>
+      <c r="B105" t="s">
+        <v>4</v>
+      </c>
+      <c r="D105" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4">
+      <c r="A106">
+        <v>104</v>
+      </c>
+      <c r="B106" t="s">
+        <v>5</v>
+      </c>
+      <c r="D106" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4">
+      <c r="A107">
+        <v>105</v>
+      </c>
+      <c r="B107" t="s">
+        <v>4</v>
+      </c>
+      <c r="D107" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>